<commit_message>
Acrescentado feature de amostragem digital ou física no FeatureModel, Product Map e Product Map - Novos Produtos
</commit_message>
<xml_diff>
--- a/Product Map/Product Map - Novos Produtos.xlsx
+++ b/Product Map/Product Map - Novos Produtos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Filipe Bomfim\Documents\UNEB\8º Semestre\Tópicos Especiais em Engenharia de Software\FeatureModel Restaurante\TEES_FeatureModelRestaurant\Product Map\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{56002699-1D09-43A7-BC60-13A6391D1A10}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{0FA16A43-926C-4DD1-940F-929D64B122D2}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8130" xr2:uid="{8EEA5BD7-CE3C-43C9-B812-895284E8C214}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="45">
   <si>
     <t>Subdomínio</t>
   </si>
@@ -51,9 +51,6 @@
     <t>Categoria</t>
   </si>
   <si>
-    <t>Mostrar Cardápio</t>
-  </si>
-  <si>
     <t>Pedido</t>
   </si>
   <si>
@@ -157,6 +154,12 @@
   </si>
   <si>
     <t xml:space="preserve">Novo Produto </t>
+  </si>
+  <si>
+    <t>Digital</t>
+  </si>
+  <si>
+    <t>Físico</t>
   </si>
 </sst>
 </file>
@@ -520,6 +523,123 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -527,123 +647,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -960,10 +963,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C82CAE47-B6DD-42A0-A8D1-E298EA86D1C1}">
-  <dimension ref="H1:L38"/>
+  <dimension ref="H1:L39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -977,27 +980,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H1" s="25" t="s">
-        <v>40</v>
-      </c>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
-      <c r="K1" s="26"/>
-      <c r="L1" s="26"/>
+      <c r="H1" s="64" t="s">
+        <v>39</v>
+      </c>
+      <c r="I1" s="65"/>
+      <c r="J1" s="65"/>
+      <c r="K1" s="65"/>
+      <c r="L1" s="65"/>
     </row>
     <row r="2" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H2" s="26"/>
-      <c r="I2" s="26"/>
-      <c r="J2" s="26"/>
-      <c r="K2" s="26"/>
-      <c r="L2" s="26"/>
+      <c r="H2" s="65"/>
+      <c r="I2" s="65"/>
+      <c r="J2" s="65"/>
+      <c r="K2" s="65"/>
+      <c r="L2" s="65"/>
     </row>
     <row r="3" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H3" s="27"/>
-      <c r="I3" s="27"/>
-      <c r="J3" s="26"/>
-      <c r="K3" s="26"/>
-      <c r="L3" s="26"/>
+      <c r="H3" s="66"/>
+      <c r="I3" s="66"/>
+      <c r="J3" s="65"/>
+      <c r="K3" s="65"/>
+      <c r="L3" s="65"/>
     </row>
     <row r="4" spans="8:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="H4" s="3" t="s">
@@ -1006,14 +1009,14 @@
       <c r="I4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="J4" s="28" t="s">
+      <c r="J4" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="K4" s="38" t="s">
+        <v>41</v>
+      </c>
+      <c r="L4" s="51" t="s">
         <v>42</v>
-      </c>
-      <c r="K4" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="L4" s="54" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="5" spans="8:12" ht="19.5" x14ac:dyDescent="0.3">
@@ -1023,23 +1026,23 @@
       <c r="I5" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="J5" s="29" t="s">
-        <v>41</v>
-      </c>
-      <c r="K5" s="42"/>
-      <c r="L5" s="55"/>
+      <c r="J5" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="K5" s="39"/>
+      <c r="L5" s="52"/>
     </row>
     <row r="6" spans="8:12" ht="19.5" x14ac:dyDescent="0.3">
       <c r="H6" s="1"/>
       <c r="I6" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="J6" s="30" t="s">
-        <v>41</v>
-      </c>
-      <c r="K6" s="43"/>
-      <c r="L6" s="56" t="s">
-        <v>41</v>
+      <c r="J6" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="K6" s="40"/>
+      <c r="L6" s="53" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="8:12" ht="19.5" x14ac:dyDescent="0.3">
@@ -1047,397 +1050,408 @@
       <c r="I7" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="J7" s="30" t="s">
-        <v>41</v>
-      </c>
-      <c r="K7" s="43"/>
-      <c r="L7" s="56"/>
+      <c r="J7" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="K7" s="40"/>
+      <c r="L7" s="53"/>
     </row>
     <row r="8" spans="8:12" ht="19.5" x14ac:dyDescent="0.3">
       <c r="H8" s="1"/>
       <c r="I8" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="J8" s="30" t="s">
-        <v>41</v>
-      </c>
-      <c r="K8" s="43" t="s">
-        <v>41</v>
-      </c>
-      <c r="L8" s="56"/>
+      <c r="J8" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="K8" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="L8" s="53"/>
     </row>
     <row r="9" spans="8:12" ht="19.5" x14ac:dyDescent="0.3">
       <c r="H9" s="1"/>
       <c r="I9" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="J9" s="30"/>
-      <c r="K9" s="43" t="s">
-        <v>41</v>
-      </c>
-      <c r="L9" s="56" t="s">
-        <v>41</v>
+      <c r="J9" s="27"/>
+      <c r="K9" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="L9" s="53" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="8:12" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="H10" s="7"/>
-      <c r="I10" s="8" t="s">
+      <c r="H10" s="1"/>
+      <c r="I10" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="J10" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="K10" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="L10" s="53"/>
+    </row>
+    <row r="11" spans="8:12" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="H11" s="7"/>
+      <c r="I11" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="J11" s="28"/>
+      <c r="K11" s="41" t="s">
+        <v>40</v>
+      </c>
+      <c r="L11" s="54" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="8:12" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="H12" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J10" s="31" t="s">
-        <v>41</v>
-      </c>
-      <c r="K10" s="44" t="s">
-        <v>41</v>
-      </c>
-      <c r="L10" s="57" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="11" spans="8:12" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="H11" s="2" t="s">
+      <c r="I12" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="I11" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="J11" s="32" t="s">
-        <v>41</v>
-      </c>
-      <c r="K11" s="45" t="s">
-        <v>41</v>
-      </c>
-      <c r="L11" s="58" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="12" spans="8:12" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="H12" s="10"/>
-      <c r="I12" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="J12" s="33" t="s">
-        <v>41</v>
-      </c>
-      <c r="K12" s="46" t="s">
-        <v>41</v>
-      </c>
-      <c r="L12" s="59" t="s">
-        <v>41</v>
+      <c r="J12" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="K12" s="42" t="s">
+        <v>40</v>
+      </c>
+      <c r="L12" s="55" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="8:12" ht="19.5" x14ac:dyDescent="0.3">
       <c r="H13" s="10"/>
       <c r="I13" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="J13" s="33" t="s">
-        <v>41</v>
-      </c>
-      <c r="K13" s="46" t="s">
-        <v>41</v>
-      </c>
-      <c r="L13" s="59" t="s">
-        <v>41</v>
+        <v>10</v>
+      </c>
+      <c r="J13" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="K13" s="43" t="s">
+        <v>40</v>
+      </c>
+      <c r="L13" s="56" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="8:12" ht="19.5" x14ac:dyDescent="0.3">
       <c r="H14" s="10"/>
       <c r="I14" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="J14" s="33"/>
-      <c r="K14" s="46"/>
-      <c r="L14" s="59" t="s">
-        <v>41</v>
+        <v>11</v>
+      </c>
+      <c r="J14" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="K14" s="43" t="s">
+        <v>40</v>
+      </c>
+      <c r="L14" s="56" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="8:12" ht="19.5" x14ac:dyDescent="0.3">
       <c r="H15" s="10"/>
       <c r="I15" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="J15" s="33" t="s">
-        <v>41</v>
-      </c>
-      <c r="K15" s="46"/>
-      <c r="L15" s="59"/>
+        <v>12</v>
+      </c>
+      <c r="J15" s="30"/>
+      <c r="K15" s="43"/>
+      <c r="L15" s="56" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="16" spans="8:12" ht="19.5" x14ac:dyDescent="0.3">
       <c r="H16" s="10"/>
       <c r="I16" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="J16" s="33"/>
-      <c r="K16" s="46" t="s">
-        <v>41</v>
-      </c>
-      <c r="L16" s="59"/>
+        <v>13</v>
+      </c>
+      <c r="J16" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="K16" s="43"/>
+      <c r="L16" s="56"/>
     </row>
     <row r="17" spans="8:12" ht="19.5" x14ac:dyDescent="0.3">
       <c r="H17" s="10"/>
       <c r="I17" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="J17" s="30"/>
+      <c r="K17" s="43" t="s">
+        <v>40</v>
+      </c>
+      <c r="L17" s="56"/>
+    </row>
+    <row r="18" spans="8:12" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="H18" s="10"/>
+      <c r="I18" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="J18" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="K18" s="43"/>
+      <c r="L18" s="56"/>
+    </row>
+    <row r="19" spans="8:12" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="H19" s="12"/>
+      <c r="I19" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="J17" s="33" t="s">
-        <v>41</v>
-      </c>
-      <c r="K17" s="46"/>
-      <c r="L17" s="59"/>
-    </row>
-    <row r="18" spans="8:12" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="H18" s="12"/>
-      <c r="I18" s="13" t="s">
+      <c r="J19" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="K19" s="44"/>
+      <c r="L19" s="57" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="8:12" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="H20" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="J18" s="34" t="s">
-        <v>41</v>
-      </c>
-      <c r="K18" s="47"/>
-      <c r="L18" s="60" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="19" spans="8:12" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="H19" s="14" t="s">
+      <c r="I20" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="I19" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="J19" s="35" t="s">
-        <v>41</v>
-      </c>
-      <c r="K19" s="48"/>
-      <c r="L19" s="61" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="20" spans="8:12" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="H20" s="16"/>
-      <c r="I20" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="J20" s="36"/>
-      <c r="K20" s="49"/>
-      <c r="L20" s="62" t="s">
-        <v>41</v>
+      <c r="J20" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="K20" s="45"/>
+      <c r="L20" s="58" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="21" spans="8:12" ht="19.5" x14ac:dyDescent="0.3">
       <c r="H21" s="16"/>
       <c r="I21" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="J21" s="36"/>
-      <c r="K21" s="49" t="s">
-        <v>41</v>
-      </c>
-      <c r="L21" s="62"/>
+        <v>19</v>
+      </c>
+      <c r="J21" s="33"/>
+      <c r="K21" s="46"/>
+      <c r="L21" s="59" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="22" spans="8:12" ht="19.5" x14ac:dyDescent="0.3">
       <c r="H22" s="16"/>
       <c r="I22" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="J22" s="36"/>
-      <c r="K22" s="49"/>
-      <c r="L22" s="62"/>
+        <v>20</v>
+      </c>
+      <c r="J22" s="33"/>
+      <c r="K22" s="46" t="s">
+        <v>40</v>
+      </c>
+      <c r="L22" s="59"/>
     </row>
     <row r="23" spans="8:12" ht="19.5" x14ac:dyDescent="0.3">
       <c r="H23" s="16"/>
       <c r="I23" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="J23" s="36" t="s">
-        <v>41</v>
-      </c>
-      <c r="K23" s="49"/>
-      <c r="L23" s="62" t="s">
-        <v>41</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="J23" s="33"/>
+      <c r="K23" s="46"/>
+      <c r="L23" s="59"/>
     </row>
     <row r="24" spans="8:12" ht="19.5" x14ac:dyDescent="0.3">
       <c r="H24" s="16"/>
       <c r="I24" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="J24" s="36" t="s">
-        <v>41</v>
-      </c>
-      <c r="K24" s="49"/>
-      <c r="L24" s="62" t="s">
-        <v>41</v>
+        <v>22</v>
+      </c>
+      <c r="J24" s="33" t="s">
+        <v>40</v>
+      </c>
+      <c r="K24" s="46"/>
+      <c r="L24" s="59" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="25" spans="8:12" ht="19.5" x14ac:dyDescent="0.3">
       <c r="H25" s="16"/>
       <c r="I25" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="J25" s="36" t="s">
-        <v>41</v>
-      </c>
-      <c r="K25" s="49"/>
-      <c r="L25" s="62" t="s">
-        <v>41</v>
+        <v>23</v>
+      </c>
+      <c r="J25" s="33" t="s">
+        <v>40</v>
+      </c>
+      <c r="K25" s="46"/>
+      <c r="L25" s="59" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="26" spans="8:12" ht="19.5" x14ac:dyDescent="0.3">
       <c r="H26" s="16"/>
       <c r="I26" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="J26" s="36" t="s">
-        <v>41</v>
-      </c>
-      <c r="K26" s="49"/>
-      <c r="L26" s="62" t="s">
-        <v>41</v>
+        <v>24</v>
+      </c>
+      <c r="J26" s="33" t="s">
+        <v>40</v>
+      </c>
+      <c r="K26" s="46"/>
+      <c r="L26" s="59" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="27" spans="8:12" ht="19.5" x14ac:dyDescent="0.3">
       <c r="H27" s="16"/>
       <c r="I27" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="J27" s="33" t="s">
+        <v>40</v>
+      </c>
+      <c r="K27" s="46"/>
+      <c r="L27" s="59" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="28" spans="8:12" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="H28" s="16"/>
+      <c r="I28" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="J28" s="33" t="s">
+        <v>40</v>
+      </c>
+      <c r="K28" s="46"/>
+      <c r="L28" s="59" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="29" spans="8:12" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="H29" s="18"/>
+      <c r="I29" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="J29" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="K29" s="47" t="s">
+        <v>40</v>
+      </c>
+      <c r="L29" s="60"/>
+    </row>
+    <row r="30" spans="8:12" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="H30" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="J27" s="36" t="s">
-        <v>41</v>
-      </c>
-      <c r="K27" s="49"/>
-      <c r="L27" s="62" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="28" spans="8:12" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="H28" s="18"/>
-      <c r="I28" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="J28" s="37" t="s">
-        <v>41</v>
-      </c>
-      <c r="K28" s="50" t="s">
-        <v>41</v>
-      </c>
-      <c r="L28" s="63"/>
-    </row>
-    <row r="29" spans="8:12" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="H29" s="20" t="s">
+      <c r="I30" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="I29" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="J29" s="38" t="s">
-        <v>41</v>
-      </c>
-      <c r="K29" s="51"/>
-      <c r="L29" s="64" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="30" spans="8:12" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="H30" s="22"/>
-      <c r="I30" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="J30" s="39" t="s">
-        <v>41</v>
-      </c>
-      <c r="K30" s="52"/>
-      <c r="L30" s="65" t="s">
-        <v>41</v>
+      <c r="J30" s="35" t="s">
+        <v>40</v>
+      </c>
+      <c r="K30" s="48"/>
+      <c r="L30" s="61" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="31" spans="8:12" ht="19.5" x14ac:dyDescent="0.3">
       <c r="H31" s="22"/>
       <c r="I31" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="J31" s="39" t="s">
-        <v>41</v>
-      </c>
-      <c r="K31" s="52"/>
-      <c r="L31" s="65" t="s">
-        <v>41</v>
+        <v>30</v>
+      </c>
+      <c r="J31" s="36" t="s">
+        <v>40</v>
+      </c>
+      <c r="K31" s="49"/>
+      <c r="L31" s="62" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="32" spans="8:12" ht="19.5" x14ac:dyDescent="0.3">
       <c r="H32" s="22"/>
       <c r="I32" s="23" t="s">
-        <v>33</v>
-      </c>
-      <c r="J32" s="39"/>
-      <c r="K32" s="52"/>
-      <c r="L32" s="65" t="s">
-        <v>41</v>
+        <v>31</v>
+      </c>
+      <c r="J32" s="36" t="s">
+        <v>40</v>
+      </c>
+      <c r="K32" s="49"/>
+      <c r="L32" s="62" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="33" spans="8:12" ht="19.5" x14ac:dyDescent="0.3">
       <c r="H33" s="22"/>
       <c r="I33" s="23" t="s">
-        <v>34</v>
-      </c>
-      <c r="J33" s="39" t="s">
-        <v>41</v>
-      </c>
-      <c r="K33" s="52"/>
-      <c r="L33" s="65"/>
+        <v>32</v>
+      </c>
+      <c r="J33" s="36"/>
+      <c r="K33" s="49"/>
+      <c r="L33" s="62" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="34" spans="8:12" ht="19.5" x14ac:dyDescent="0.3">
       <c r="H34" s="22"/>
       <c r="I34" s="23" t="s">
-        <v>35</v>
-      </c>
-      <c r="J34" s="39"/>
-      <c r="K34" s="52"/>
-      <c r="L34" s="65"/>
+        <v>33</v>
+      </c>
+      <c r="J34" s="36" t="s">
+        <v>40</v>
+      </c>
+      <c r="K34" s="49"/>
+      <c r="L34" s="62"/>
     </row>
     <row r="35" spans="8:12" ht="19.5" x14ac:dyDescent="0.3">
       <c r="H35" s="22"/>
       <c r="I35" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="J35" s="39"/>
-      <c r="K35" s="52"/>
-      <c r="L35" s="65" t="s">
-        <v>41</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="J35" s="36"/>
+      <c r="K35" s="49"/>
+      <c r="L35" s="62"/>
     </row>
     <row r="36" spans="8:12" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="H36" s="23"/>
+      <c r="H36" s="22"/>
       <c r="I36" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="J36" s="39"/>
-      <c r="K36" s="52"/>
-      <c r="L36" s="65" t="s">
-        <v>41</v>
+        <v>35</v>
+      </c>
+      <c r="J36" s="36"/>
+      <c r="K36" s="49"/>
+      <c r="L36" s="62" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="37" spans="8:12" ht="19.5" x14ac:dyDescent="0.3">
       <c r="H37" s="23"/>
       <c r="I37" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="J37" s="36"/>
+      <c r="K37" s="49"/>
+      <c r="L37" s="62" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="38" spans="8:12" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="H38" s="23"/>
+      <c r="I38" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="J38" s="36"/>
+      <c r="K38" s="49"/>
+      <c r="L38" s="62" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="39" spans="8:12" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="H39" s="24"/>
+      <c r="I39" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="J37" s="39"/>
-      <c r="K37" s="52"/>
-      <c r="L37" s="65" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="38" spans="8:12" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="H38" s="24"/>
-      <c r="I38" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="J38" s="40" t="s">
-        <v>41</v>
-      </c>
-      <c r="K38" s="53"/>
-      <c r="L38" s="66" t="s">
-        <v>41</v>
+      <c r="J39" s="37" t="s">
+        <v>40</v>
+      </c>
+      <c r="K39" s="50"/>
+      <c r="L39" s="63" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>